<commit_message>
fix(p29): 严格按 config.output.final_ppt 生成最终PPT 并同步文档
</commit_message>
<xml_diff>
--- a/charts/p29/p29_data.xlsx
+++ b/charts/p29/p29_data.xlsx
@@ -527,25 +527,25 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
         <v>6</v>
       </c>
-      <c r="C2" t="n">
-        <v>5</v>
-      </c>
       <c r="D2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F2" t="n">
         <v>4</v>
       </c>
       <c r="G2" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -555,25 +555,25 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" t="n">
+        <v>22</v>
+      </c>
+      <c r="D3" t="n">
         <v>4</v>
       </c>
-      <c r="C3" t="n">
+      <c r="E3" t="n">
         <v>4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="H3" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -583,25 +583,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C4" t="n">
+        <v>15</v>
+      </c>
+      <c r="D4" t="n">
         <v>2</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
         <v>0</v>
       </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
       <c r="G4" t="n">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="H4" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -611,25 +611,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="H5" t="n">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -639,25 +639,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -667,25 +667,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E7" t="n">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="H7" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -699,7 +699,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -771,13 +771,13 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>-0.66</v>
+        <v>-0.45</v>
       </c>
     </row>
     <row r="4">
@@ -797,13 +797,13 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>5230</v>
+        <v>746</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>-0.19</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="5">
@@ -829,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>1.18</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="6">
@@ -849,13 +849,13 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>284</v>
+        <v>545</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>0.45</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="7">
@@ -875,13 +875,13 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>1.65</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="8">
@@ -927,13 +927,13 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>1163</v>
+        <v>615</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>4.08</v>
+        <v>4.13</v>
       </c>
     </row>
     <row r="10">
@@ -953,13 +953,13 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>-0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -979,13 +979,13 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>1416</v>
+        <v>158</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="4" t="n">
-        <v>-0.19</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="12">
@@ -1031,13 +1031,13 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="4" t="n">
-        <v>-0.14</v>
+        <v>-0.16</v>
       </c>
     </row>
     <row r="14">
@@ -1109,39 +1109,39 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>134</v>
+        <v>41</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F16" s="4" t="n">
-        <v>2.96</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Online News</t>
+          <t>Forum</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>ASUS</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>comment</t>
+          <t>forum</t>
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="E17" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F17" s="4" t="n">
-        <v>-0.49</v>
+        <v>-0.58</v>
       </c>
     </row>
     <row r="18">
@@ -1152,7 +1152,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Acer</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -1161,13 +1161,13 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>33</v>
+        <v>191</v>
       </c>
       <c r="E18" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>-0.58</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="19">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1187,13 +1187,13 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>227</v>
+        <v>306</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>0.85</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="20">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1213,13 +1213,13 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>305</v>
+        <v>47</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>0.2</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>Apple</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1239,13 +1239,13 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="4" t="n">
-        <v>0.61</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="22">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Lenovo</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1265,13 +1265,13 @@
         </is>
       </c>
       <c r="D22" s="4" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F22" s="4" t="n">
-        <v>-0.13</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="23">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>Lenovo</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1291,39 +1291,39 @@
         </is>
       </c>
       <c r="D23" s="4" t="n">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="E23" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F23" s="4" t="n">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Forum</t>
+          <t>Online News</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>ASUS</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>forum</t>
+          <t>frontpage</t>
         </is>
       </c>
       <c r="D24" s="4" t="n">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="E24" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F24" s="4" t="n">
-        <v>0.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Acer</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1343,13 +1343,13 @@
         </is>
       </c>
       <c r="D25" s="4" t="n">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="E25" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F25" s="4" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="26">
@@ -1360,7 +1360,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1369,13 +1369,13 @@
         </is>
       </c>
       <c r="D26" s="4" t="n">
-        <v>811</v>
+        <v>40</v>
       </c>
       <c r="E26" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F26" s="4" t="n">
-        <v>-0.28</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="27">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -1395,13 +1395,13 @@
         </is>
       </c>
       <c r="D27" s="4" t="n">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="E27" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F27" s="4" t="n">
-        <v>0.62</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="28">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>Apple</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1421,13 +1421,13 @@
         </is>
       </c>
       <c r="D28" s="4" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F28" s="4" t="n">
-        <v>0.11</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="29">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Lenovo</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -1447,13 +1447,13 @@
         </is>
       </c>
       <c r="D29" s="4" t="n">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E29" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F29" s="4" t="n">
-        <v>0.55</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="30">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>Lenovo</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1473,39 +1473,39 @@
         </is>
       </c>
       <c r="D30" s="4" t="n">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E30" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F30" s="4" t="n">
-        <v>0.62</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>Online News</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>ASUS</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>frontpage</t>
+          <t>instagram</t>
         </is>
       </c>
       <c r="D31" s="4" t="n">
-        <v>473</v>
+        <v>15</v>
       </c>
       <c r="E31" s="4" t="n">
-        <v>0</v>
+        <v>2566</v>
       </c>
       <c r="F31" s="4" t="n">
-        <v>0.07000000000000001</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="32">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Acer</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1525,13 +1525,13 @@
         </is>
       </c>
       <c r="D32" s="4" t="n">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="E32" s="4" t="n">
-        <v>2580</v>
+        <v>9181</v>
       </c>
       <c r="F32" s="4" t="n">
-        <v>1.56</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="33">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -1551,13 +1551,13 @@
         </is>
       </c>
       <c r="D33" s="4" t="n">
-        <v>453</v>
+        <v>57</v>
       </c>
       <c r="E33" s="4" t="n">
-        <v>45047</v>
+        <v>546</v>
       </c>
       <c r="F33" s="4" t="n">
-        <v>0.99</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="34">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1577,13 +1577,13 @@
         </is>
       </c>
       <c r="D34" s="4" t="n">
-        <v>56</v>
+        <v>403</v>
       </c>
       <c r="E34" s="4" t="n">
-        <v>536</v>
+        <v>18197</v>
       </c>
       <c r="F34" s="4" t="n">
-        <v>0.25</v>
+        <v>1.93</v>
       </c>
     </row>
     <row r="35">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>Apple</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -1603,13 +1603,13 @@
         </is>
       </c>
       <c r="D35" s="4" t="n">
-        <v>160</v>
+        <v>3</v>
       </c>
       <c r="E35" s="4" t="n">
-        <v>11955</v>
+        <v>139</v>
       </c>
       <c r="F35" s="4" t="n">
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Lenovo</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1629,13 +1629,13 @@
         </is>
       </c>
       <c r="D36" s="4" t="n">
-        <v>3</v>
+        <v>379</v>
       </c>
       <c r="E36" s="4" t="n">
-        <v>139</v>
+        <v>24794</v>
       </c>
       <c r="F36" s="4" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="37">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Lenovo</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1655,39 +1655,39 @@
         </is>
       </c>
       <c r="D37" s="4" t="n">
-        <v>379</v>
+        <v>9</v>
       </c>
       <c r="E37" s="4" t="n">
-        <v>24794</v>
+        <v>2735</v>
       </c>
       <c r="F37" s="4" t="n">
-        <v>0.16</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>Instagram</t>
+          <t>X</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>ASUS</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>instagram</t>
+          <t>twitter</t>
         </is>
       </c>
       <c r="D38" s="4" t="n">
-        <v>360</v>
+        <v>37</v>
       </c>
       <c r="E38" s="4" t="n">
-        <v>9446</v>
+        <v>6</v>
       </c>
       <c r="F38" s="4" t="n">
-        <v>1.25</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="39">
@@ -1698,7 +1698,7 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Acer</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1707,13 +1707,13 @@
         </is>
       </c>
       <c r="D39" s="4" t="n">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="E39" s="4" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F39" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="40">
@@ -1724,7 +1724,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1733,13 +1733,13 @@
         </is>
       </c>
       <c r="D40" s="4" t="n">
-        <v>826</v>
+        <v>142</v>
       </c>
       <c r="E40" s="4" t="n">
-        <v>206</v>
+        <v>17</v>
       </c>
       <c r="F40" s="4" t="n">
-        <v>-0</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="41">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1759,10 +1759,10 @@
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="E41" s="4" t="n">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="F41" s="4" t="n">
         <v>0.17</v>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>Apple</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1785,13 +1785,13 @@
         </is>
       </c>
       <c r="D42" s="4" t="n">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="E42" s="4" t="n">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F42" s="4" t="n">
-        <v>0.17</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="43">
@@ -1802,7 +1802,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Lenovo</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -1811,13 +1811,13 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>74</v>
+        <v>429</v>
       </c>
       <c r="E43" s="4" t="n">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="F43" s="4" t="n">
-        <v>-0.18</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="44">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>Lenovo</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -1837,39 +1837,39 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>429</v>
+        <v>66</v>
       </c>
       <c r="E44" s="4" t="n">
-        <v>126</v>
+        <v>10</v>
       </c>
       <c r="F44" s="4" t="n">
-        <v>1.12</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>YouTube</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>ASUS</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>twitter</t>
+          <t>video</t>
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>751</v>
+        <v>205</v>
       </c>
       <c r="E45" s="4" t="n">
-        <v>179</v>
+        <v>12424</v>
       </c>
       <c r="F45" s="4" t="n">
-        <v>0.19</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="46">
@@ -1880,7 +1880,7 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Acer</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -1889,13 +1889,13 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>871</v>
+        <v>443</v>
       </c>
       <c r="E46" s="4" t="n">
-        <v>13564</v>
+        <v>29862</v>
       </c>
       <c r="F46" s="4" t="n">
-        <v>0.64</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="47">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
@@ -1915,13 +1915,13 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>20574</v>
+        <v>6445</v>
       </c>
       <c r="E47" s="4" t="n">
-        <v>462241</v>
+        <v>96421</v>
       </c>
       <c r="F47" s="4" t="n">
-        <v>-0.21</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="48">
@@ -1932,7 +1932,7 @@
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Dell</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -1941,13 +1941,13 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>6443</v>
+        <v>937</v>
       </c>
       <c r="E48" s="4" t="n">
-        <v>95587</v>
+        <v>10043</v>
       </c>
       <c r="F48" s="4" t="n">
-        <v>1.22</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="49">
@@ -1958,7 +1958,7 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>Dell</t>
+          <t>Apple</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -1967,13 +1967,13 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>883</v>
+        <v>903</v>
       </c>
       <c r="E49" s="4" t="n">
-        <v>9471</v>
+        <v>6383</v>
       </c>
       <c r="F49" s="4" t="n">
-        <v>1.05</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="50">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Lenovo</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
@@ -1993,13 +1993,13 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>890</v>
+        <v>3153</v>
       </c>
       <c r="E50" s="4" t="n">
-        <v>6035</v>
+        <v>36391</v>
       </c>
       <c r="F50" s="4" t="n">
-        <v>1.35</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="51">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Lenovo</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
@@ -2019,39 +2019,13 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>3150</v>
+        <v>524</v>
       </c>
       <c r="E51" s="4" t="n">
-        <v>35898</v>
+        <v>52169</v>
       </c>
       <c r="F51" s="4" t="n">
-        <v>1.19</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="3" t="inlineStr">
-        <is>
-          <t>YouTube</t>
-        </is>
-      </c>
-      <c r="B52" s="3" t="inlineStr">
-        <is>
-          <t>Samsung</t>
-        </is>
-      </c>
-      <c r="C52" s="3" t="inlineStr">
-        <is>
-          <t>video</t>
-        </is>
-      </c>
-      <c r="D52" s="4" t="n">
-        <v>6176</v>
-      </c>
-      <c r="E52" s="4" t="n">
-        <v>82800</v>
-      </c>
-      <c r="F52" s="4" t="n">
-        <v>1.75</v>
+        <v>0.61</v>
       </c>
     </row>
   </sheetData>
@@ -2132,10 +2106,10 @@
         <v>56</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>894</v>
+        <v>796</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>6.3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -2150,13 +2124,13 @@
         </is>
       </c>
       <c r="C4" s="4" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>894</v>
+        <v>796</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>5.1</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="5">
@@ -2174,10 +2148,10 @@
         <v>78</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>894</v>
+        <v>796</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>8.699999999999999</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -2192,13 +2166,13 @@
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>894</v>
+        <v>796</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>34.1</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="7">
@@ -2216,10 +2190,10 @@
         <v>33</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>894</v>
+        <v>796</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>3.7</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="8">
@@ -2234,13 +2208,13 @@
         </is>
       </c>
       <c r="C8" s="4" t="n">
-        <v>227</v>
+        <v>191</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>894</v>
+        <v>796</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>25.4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
@@ -2255,13 +2229,13 @@
         </is>
       </c>
       <c r="C9" s="4" t="n">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>894</v>
+        <v>796</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>16.7</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="10">
@@ -2279,10 +2253,10 @@
         <v>333</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>8674</v>
+        <v>2717</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>3.8</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="11">
@@ -2297,13 +2271,13 @@
         </is>
       </c>
       <c r="C11" s="4" t="n">
-        <v>320</v>
+        <v>604</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>8674</v>
+        <v>2717</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>3.7</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="12">
@@ -2318,13 +2292,13 @@
         </is>
       </c>
       <c r="C12" s="4" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>8674</v>
+        <v>2717</v>
       </c>
       <c r="E12" s="4" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="13">
@@ -2339,13 +2313,13 @@
         </is>
       </c>
       <c r="C13" s="4" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>8674</v>
+        <v>2717</v>
       </c>
       <c r="E13" s="4" t="n">
-        <v>1.4</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="14">
@@ -2360,13 +2334,13 @@
         </is>
       </c>
       <c r="C14" s="4" t="n">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>8674</v>
+        <v>2717</v>
       </c>
       <c r="E14" s="4" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -2381,13 +2355,13 @@
         </is>
       </c>
       <c r="C15" s="4" t="n">
-        <v>6109</v>
+        <v>859</v>
       </c>
       <c r="D15" s="4" t="n">
-        <v>8674</v>
+        <v>2717</v>
       </c>
       <c r="E15" s="4" t="n">
-        <v>70.40000000000001</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="16">
@@ -2402,13 +2376,13 @@
         </is>
       </c>
       <c r="C16" s="4" t="n">
-        <v>1636</v>
+        <v>673</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>8674</v>
+        <v>2717</v>
       </c>
       <c r="E16" s="4" t="n">
-        <v>18.9</v>
+        <v>24.8</v>
       </c>
     </row>
     <row r="17">
@@ -2426,10 +2400,10 @@
         <v>99</v>
       </c>
       <c r="D17" s="4" t="n">
-        <v>1714</v>
+        <v>372</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>5.8</v>
+        <v>26.6</v>
       </c>
     </row>
     <row r="18">
@@ -2444,13 +2418,13 @@
         </is>
       </c>
       <c r="C18" s="4" t="n">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>1714</v>
+        <v>372</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>2</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="19">
@@ -2468,10 +2442,10 @@
         <v>7</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>1714</v>
+        <v>372</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>0.4</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="20">
@@ -2489,10 +2463,10 @@
         <v>11</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>1714</v>
+        <v>372</v>
       </c>
       <c r="E20" s="4" t="n">
-        <v>0.6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -2507,13 +2481,13 @@
         </is>
       </c>
       <c r="C21" s="4" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>1714</v>
+        <v>372</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="22">
@@ -2528,13 +2502,13 @@
         </is>
       </c>
       <c r="C22" s="4" t="n">
-        <v>1416</v>
+        <v>158</v>
       </c>
       <c r="D22" s="4" t="n">
-        <v>1714</v>
+        <v>372</v>
       </c>
       <c r="E22" s="4" t="n">
-        <v>82.59999999999999</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="23">
@@ -2549,13 +2523,13 @@
         </is>
       </c>
       <c r="C23" s="4" t="n">
-        <v>134</v>
+        <v>41</v>
       </c>
       <c r="D23" s="4" t="n">
-        <v>1714</v>
+        <v>372</v>
       </c>
       <c r="E23" s="4" t="n">
-        <v>7.8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
@@ -2573,10 +2547,10 @@
         <v>429</v>
       </c>
       <c r="D24" s="4" t="n">
-        <v>2311</v>
+        <v>917</v>
       </c>
       <c r="E24" s="4" t="n">
-        <v>18.6</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="25">
@@ -2591,13 +2565,13 @@
         </is>
       </c>
       <c r="C25" s="4" t="n">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>2311</v>
+        <v>917</v>
       </c>
       <c r="E25" s="4" t="n">
-        <v>2.3</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="26">
@@ -2615,10 +2589,10 @@
         <v>74</v>
       </c>
       <c r="D26" s="4" t="n">
-        <v>2311</v>
+        <v>917</v>
       </c>
       <c r="E26" s="4" t="n">
-        <v>3.2</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="27">
@@ -2633,13 +2607,13 @@
         </is>
       </c>
       <c r="C27" s="4" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D27" s="4" t="n">
-        <v>2311</v>
+        <v>917</v>
       </c>
       <c r="E27" s="4" t="n">
-        <v>6.1</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="28">
@@ -2654,13 +2628,13 @@
         </is>
       </c>
       <c r="C28" s="4" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D28" s="4" t="n">
-        <v>2311</v>
+        <v>917</v>
       </c>
       <c r="E28" s="4" t="n">
-        <v>1.6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -2675,13 +2649,13 @@
         </is>
       </c>
       <c r="C29" s="4" t="n">
-        <v>826</v>
+        <v>97</v>
       </c>
       <c r="D29" s="4" t="n">
-        <v>2311</v>
+        <v>917</v>
       </c>
       <c r="E29" s="4" t="n">
-        <v>35.7</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="30">
@@ -2696,13 +2670,13 @@
         </is>
       </c>
       <c r="C30" s="4" t="n">
-        <v>751</v>
+        <v>66</v>
       </c>
       <c r="D30" s="4" t="n">
-        <v>2311</v>
+        <v>917</v>
       </c>
       <c r="E30" s="4" t="n">
-        <v>32.5</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="31">
@@ -2720,10 +2694,10 @@
         <v>379</v>
       </c>
       <c r="D31" s="4" t="n">
-        <v>1514</v>
+        <v>895</v>
       </c>
       <c r="E31" s="4" t="n">
-        <v>25</v>
+        <v>42.3</v>
       </c>
     </row>
     <row r="32">
@@ -2738,13 +2712,13 @@
         </is>
       </c>
       <c r="C32" s="4" t="n">
-        <v>160</v>
+        <v>403</v>
       </c>
       <c r="D32" s="4" t="n">
-        <v>1514</v>
+        <v>895</v>
       </c>
       <c r="E32" s="4" t="n">
-        <v>10.6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33">
@@ -2762,10 +2736,10 @@
         <v>3</v>
       </c>
       <c r="D33" s="4" t="n">
-        <v>1514</v>
+        <v>895</v>
       </c>
       <c r="E33" s="4" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="34">
@@ -2780,13 +2754,13 @@
         </is>
       </c>
       <c r="C34" s="4" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D34" s="4" t="n">
-        <v>1514</v>
+        <v>895</v>
       </c>
       <c r="E34" s="4" t="n">
-        <v>3.7</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="35">
@@ -2801,13 +2775,13 @@
         </is>
       </c>
       <c r="C35" s="4" t="n">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="D35" s="4" t="n">
-        <v>1514</v>
+        <v>895</v>
       </c>
       <c r="E35" s="4" t="n">
-        <v>6.8</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="36">
@@ -2822,13 +2796,13 @@
         </is>
       </c>
       <c r="C36" s="4" t="n">
-        <v>453</v>
+        <v>29</v>
       </c>
       <c r="D36" s="4" t="n">
-        <v>1514</v>
+        <v>895</v>
       </c>
       <c r="E36" s="4" t="n">
-        <v>29.9</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="37">
@@ -2843,13 +2817,13 @@
         </is>
       </c>
       <c r="C37" s="4" t="n">
-        <v>360</v>
+        <v>9</v>
       </c>
       <c r="D37" s="4" t="n">
-        <v>1514</v>
+        <v>895</v>
       </c>
       <c r="E37" s="4" t="n">
-        <v>23.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -2864,13 +2838,13 @@
         </is>
       </c>
       <c r="C38" s="4" t="n">
-        <v>3150</v>
+        <v>3153</v>
       </c>
       <c r="D38" s="4" t="n">
-        <v>38987</v>
+        <v>12610</v>
       </c>
       <c r="E38" s="4" t="n">
-        <v>8.1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39">
@@ -2885,13 +2859,13 @@
         </is>
       </c>
       <c r="C39" s="4" t="n">
-        <v>883</v>
+        <v>937</v>
       </c>
       <c r="D39" s="4" t="n">
-        <v>38987</v>
+        <v>12610</v>
       </c>
       <c r="E39" s="4" t="n">
-        <v>2.3</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="40">
@@ -2906,13 +2880,13 @@
         </is>
       </c>
       <c r="C40" s="4" t="n">
-        <v>890</v>
+        <v>903</v>
       </c>
       <c r="D40" s="4" t="n">
-        <v>38987</v>
+        <v>12610</v>
       </c>
       <c r="E40" s="4" t="n">
-        <v>2.3</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="41">
@@ -2927,13 +2901,13 @@
         </is>
       </c>
       <c r="C41" s="4" t="n">
-        <v>6443</v>
+        <v>6445</v>
       </c>
       <c r="D41" s="4" t="n">
-        <v>38987</v>
+        <v>12610</v>
       </c>
       <c r="E41" s="4" t="n">
-        <v>16.5</v>
+        <v>51.1</v>
       </c>
     </row>
     <row r="42">
@@ -2948,13 +2922,13 @@
         </is>
       </c>
       <c r="C42" s="4" t="n">
-        <v>871</v>
+        <v>205</v>
       </c>
       <c r="D42" s="4" t="n">
-        <v>38987</v>
+        <v>12610</v>
       </c>
       <c r="E42" s="4" t="n">
-        <v>2.2</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="43">
@@ -2969,13 +2943,13 @@
         </is>
       </c>
       <c r="C43" s="4" t="n">
-        <v>20574</v>
+        <v>443</v>
       </c>
       <c r="D43" s="4" t="n">
-        <v>38987</v>
+        <v>12610</v>
       </c>
       <c r="E43" s="4" t="n">
-        <v>52.8</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="44">
@@ -2990,13 +2964,13 @@
         </is>
       </c>
       <c r="C44" s="4" t="n">
-        <v>6176</v>
+        <v>524</v>
       </c>
       <c r="D44" s="4" t="n">
-        <v>38987</v>
+        <v>12610</v>
       </c>
       <c r="E44" s="4" t="n">
-        <v>15.8</v>
+        <v>4.2</v>
       </c>
     </row>
   </sheetData>
@@ -3057,10 +3031,10 @@
         </is>
       </c>
       <c r="B3" s="4" t="n">
-        <v>4446</v>
+        <v>4449</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -3070,10 +3044,10 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>1498</v>
+        <v>2118</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -3083,10 +3057,10 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>1151</v>
+        <v>1166</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -3096,10 +3070,10 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>7074</v>
+        <v>7080</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
@@ -3109,7 +3083,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>1114</v>
+        <v>319</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>2</v>
@@ -3122,10 +3096,10 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>29605</v>
+        <v>1777</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -3135,10 +3109,10 @@
         </is>
       </c>
       <c r="B9" s="4" t="n">
-        <v>9206</v>
+        <v>1398</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>